<commit_message>
atualizacao sabao em barra
</commit_message>
<xml_diff>
--- a/pages/BA_ssoservi_cservico_csala.xlsx
+++ b/pages/BA_ssoservi_cservico_csala.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel.viana\Documents\GitHub\portal-suprimentos\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F206A36-C377-4156-A7D8-992437CAF727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73254B17-438F-4355-9544-3E6F4925769F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{66DD5035-C496-4A33-BA22-CD402935C2B8}"/>
   </bookViews>
@@ -434,9 +434,6 @@
     <t>MIL</t>
   </si>
   <si>
-    <t>SABAO EM BARRA - PACOTE C/5</t>
-  </si>
-  <si>
     <t>S010046</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>AGULHA IM - CALIBRE 40X1,20MM</t>
+  </si>
+  <si>
+    <t>SABAO EM BARRA - 200G - 200G</t>
   </si>
 </sst>
 </file>
@@ -773,16 +773,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Ruim" xfId="1" builtinId="27"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF0070C0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <border>
         <bottom style="thin">
@@ -1116,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A369FB58-D533-46A6-B5FA-793763E80E34}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,13 +1149,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="D3" s="5">
         <v>118</v>
@@ -1172,7 +1163,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>126</v>
@@ -1186,7 +1177,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>125</v>
@@ -1228,13 +1219,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>177</v>
       </c>
       <c r="D8" s="4">
         <v>1208</v>
@@ -1354,7 +1345,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>125</v>
@@ -1368,13 +1359,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="D18" s="4">
         <v>1184</v>
@@ -1424,7 +1415,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>126</v>
@@ -1433,12 +1424,12 @@
         <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>126</v>
@@ -1522,13 +1513,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" s="5">
         <v>874</v>
@@ -1550,13 +1541,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D31" s="4">
         <v>1160</v>
@@ -1578,7 +1569,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>125</v>
@@ -1592,7 +1583,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>125</v>
@@ -1606,7 +1597,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>125</v>
@@ -1620,7 +1611,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>125</v>
@@ -1634,7 +1625,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>125</v>
@@ -1648,7 +1639,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>125</v>
@@ -1662,7 +1653,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>125</v>
@@ -1676,7 +1667,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>125</v>
@@ -1690,7 +1681,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>125</v>
@@ -1760,7 +1751,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>125</v>
@@ -1774,13 +1765,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="D47" s="4">
         <v>750</v>
@@ -1830,13 +1821,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" s="4">
         <v>272</v>
@@ -1844,7 +1835,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>125</v>
@@ -1872,7 +1863,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>126</v>
@@ -1900,13 +1891,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="D56" s="4">
         <v>116</v>
@@ -1914,7 +1905,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>125</v>
@@ -1928,7 +1919,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>126</v>
@@ -1937,18 +1928,18 @@
         <v>98</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="D59" s="4">
         <v>1164</v>
@@ -1984,7 +1975,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>125</v>
@@ -1998,7 +1989,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>125</v>
@@ -2026,13 +2017,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D65" s="4">
         <v>33</v>
@@ -2040,13 +2031,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D66" s="4">
         <v>33</v>
@@ -2054,13 +2045,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="D67" s="4">
         <v>32</v>
@@ -2068,13 +2059,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="D68" s="4">
         <v>33</v>
@@ -2082,13 +2073,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D69" s="4">
         <v>32</v>
@@ -2096,13 +2087,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D70" s="4">
         <v>31</v>
@@ -2124,13 +2115,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D72" s="4">
         <v>1181</v>
@@ -2138,13 +2129,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D73" s="4">
         <v>874</v>
@@ -2152,13 +2143,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="D74" s="4">
         <v>1172</v>
@@ -2166,13 +2157,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D75" s="4">
         <v>1173</v>
@@ -2180,13 +2171,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D76" s="4">
         <v>1174</v>
@@ -2208,21 +2199,21 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="4" t="s">
+      <c r="D78" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>125</v>
@@ -2236,7 +2227,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>125</v>
@@ -2278,7 +2269,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>127</v>
@@ -2376,13 +2367,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D90" s="4">
         <v>1457</v>
@@ -2390,7 +2381,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>125</v>
@@ -2404,7 +2395,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>125</v>
@@ -2418,7 +2409,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>125</v>
@@ -2432,16 +2423,16 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="D94" s="4">
-        <v>884</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,7 +2465,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>127</v>
@@ -2488,7 +2479,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>127</v>
@@ -2502,7 +2493,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>127</v>
@@ -2614,7 +2605,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>125</v>
@@ -2642,7 +2633,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>126</v>
@@ -2656,16 +2647,16 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>129</v>
       </c>
       <c r="C110" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D110" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2684,7 +2675,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>125</v>
@@ -2703,18 +2694,13 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="2" priority="59">
+    <cfRule type="expression" dxfId="1" priority="59">
       <formula>$E1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:D32 A37:D112">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="A2:D112">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:D36">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A33))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>